<commit_message>
Updated break if there is 0 count or more than 500
</commit_message>
<xml_diff>
--- a/Data/SourceData.xlsx
+++ b/Data/SourceData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Windows\eclipse-workspace\QATasks\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Windows\eclipse-workspace\QATasks_DockerParallel\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45D5AEA7-351F-40CD-9B9B-10607C382A12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{067515BC-6758-4AA3-9AC9-4D5EC1366BF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,12 +25,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Molecule</t>
   </si>
   <si>
-    <t>CEFTRIAXONE 1GM</t>
+    <t>Adrenaline (1Mg)</t>
+  </si>
+  <si>
+    <t>Acyclovir (800Mg)</t>
+  </si>
+  <si>
+    <t>Acetylcysteine-200Mg</t>
   </si>
 </sst>
 </file>
@@ -363,10 +369,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -384,6 +390,16 @@
         <v>1</v>
       </c>
     </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>